<commit_message>
Fix HTML report showing zero passed count
Root cause: Status value mismatch between test automation and reporter
- testzen_automation.py sets status as 'PASSED'/'FAILED'
- professional_reporter.py was checking for 'PASS'/'FAIL'
- This mismatch prevented counters from incrementing

Fix: Updated professional_reporter.py to check for 'PASSED'/'FAILED'
Result: HTML report now correctly displays passed/failed test counts
</commit_message>
<xml_diff>
--- a/tests/android/billing/Payment_Form_Validation_Test.xlsx
+++ b/tests/android/billing/Payment_Form_Validation_Test.xlsx
@@ -1125,7 +1125,7 @@
       </c>
       <c r="B6" s="45" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-10-14</t>
         </is>
       </c>
     </row>
@@ -1137,7 +1137,7 @@
       </c>
       <c r="B7" s="45" t="inlineStr">
         <is>
-          <t>109</t>
+          <t>206</t>
         </is>
       </c>
     </row>

</xml_diff>